<commit_message>
create login form && main form
</commit_message>
<xml_diff>
--- a/cafe_management/src/data/dataTemplate.xlsx
+++ b/cafe_management/src/data/dataTemplate.xlsx
@@ -5,20 +5,21 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SPKT\doAn\python\CafeManagement\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SPKT\HocKy3\Python\Projects\python\cafe_management\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{223A5C71-F9DC-4FC2-ACC1-D2AFDCEEF35E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D383CD-0755-40D4-A238-C20E6102BB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{CA152D2A-739E-48A0-B88A-38360C316E83}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CA152D2A-739E-48A0-B88A-38360C316E83}"/>
   </bookViews>
   <sheets>
-    <sheet name="Category" sheetId="1" r:id="rId1"/>
-    <sheet name="Product" sheetId="2" r:id="rId2"/>
-    <sheet name="Staff" sheetId="3" r:id="rId3"/>
-    <sheet name="Customer" sheetId="4" r:id="rId4"/>
-    <sheet name="Order" sheetId="5" r:id="rId5"/>
-    <sheet name="Invoice" sheetId="6" r:id="rId6"/>
+    <sheet name="Users" sheetId="7" r:id="rId1"/>
+    <sheet name="Category" sheetId="1" r:id="rId2"/>
+    <sheet name="Product" sheetId="2" r:id="rId3"/>
+    <sheet name="Staff" sheetId="3" r:id="rId4"/>
+    <sheet name="Customer" sheetId="4" r:id="rId5"/>
+    <sheet name="Order" sheetId="5" r:id="rId6"/>
+    <sheet name="Invoice" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>maLSP</t>
   </si>
@@ -83,6 +84,30 @@
   </si>
   <si>
     <t>Sinh tố</t>
+  </si>
+  <si>
+    <t>Username</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>user1</t>
+  </si>
+  <si>
+    <t>pass1</t>
+  </si>
+  <si>
+    <t>user2</t>
+  </si>
+  <si>
+    <t>pass2</t>
+  </si>
+  <si>
+    <t>user3</t>
+  </si>
+  <si>
+    <t>pass3</t>
   </si>
 </sst>
 </file>
@@ -93,13 +118,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Arial"/>
+      <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -124,8 +149,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -459,6 +487,53 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F06D26A0-5F7D-4EBF-91E8-227E0179787A}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9718F82F-85C8-444B-93A7-82421BD9F661}">
   <dimension ref="A1:B1"/>
   <sheetViews>
@@ -466,9 +541,9 @@
       <selection sqref="A1:B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -481,17 +556,17 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BAB2B3-C2D3-4450-BB20-1F6642B07592}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -499,7 +574,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -507,7 +582,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -515,7 +590,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -523,7 +598,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -531,7 +606,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -546,43 +621,43 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C789E50B-4594-4866-AF70-8D33ED12D6DB}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8174A26E-4197-4AE7-917B-D5BB0CEEF8C7}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D9BB1D5-0C7B-4360-AEDB-70420BC71468}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53C0D48F-15D6-4340-93B2-87133DE6958D}">
   <dimension ref="A1"/>
   <sheetViews>
@@ -590,7 +665,7 @@
       <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Sửa cấu trúc file model và service login
</commit_message>
<xml_diff>
--- a/cafe_management/src/data/dataTemplate.xlsx
+++ b/cafe_management/src/data/dataTemplate.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SPKT\HocKy3\Python\Projects\python\cafe_management\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D383CD-0755-40D4-A238-C20E6102BB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF27BFE-823E-4FCE-A754-702AB64CBE66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CA152D2A-739E-48A0-B88A-38360C316E83}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{CA152D2A-739E-48A0-B88A-38360C316E83}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="7" r:id="rId1"/>
     <sheet name="Category" sheetId="1" r:id="rId2"/>
-    <sheet name="Product" sheetId="2" r:id="rId3"/>
+    <sheet name="Products" sheetId="2" r:id="rId3"/>
     <sheet name="Staff" sheetId="3" r:id="rId4"/>
     <sheet name="Customer" sheetId="4" r:id="rId5"/>
     <sheet name="Order" sheetId="5" r:id="rId6"/>
@@ -50,12 +50,6 @@
     <t>tenLSP</t>
   </si>
   <si>
-    <t>maSP</t>
-  </si>
-  <si>
-    <t>tenSP</t>
-  </si>
-  <si>
     <t>LSP0001</t>
   </si>
   <si>
@@ -108,6 +102,12 @@
   </si>
   <si>
     <t>pass3</t>
+  </si>
+  <si>
+    <t>idProduct</t>
+  </si>
+  <si>
+    <t>nameProduct</t>
   </si>
 </sst>
 </file>
@@ -490,42 +490,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F06D26A0-5F7D-4EBF-91E8-227E0179787A}">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -538,7 +538,7 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -560,58 +560,61 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BAB2B3-C2D3-4450-BB20-1F6642B07592}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="11.88671875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added models and init files
</commit_message>
<xml_diff>
--- a/cafe_management/src/data/dataTemplate.xlsx
+++ b/cafe_management/src/data/dataTemplate.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SPKT\HocKy3\Python\Projects\python\cafe_management\src\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AnhHa\source\repos\python\cafe_management\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11D383CD-0755-40D4-A238-C20E6102BB42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFB1D576-10B0-4452-9018-C7D5D44B4200}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CA152D2A-739E-48A0-B88A-38360C316E83}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{CA152D2A-739E-48A0-B88A-38360C316E83}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="7" r:id="rId1"/>
@@ -42,19 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
-  <si>
-    <t>maLSP</t>
-  </si>
-  <si>
-    <t>tenLSP</t>
-  </si>
-  <si>
-    <t>maSP</t>
-  </si>
-  <si>
-    <t>tenSP</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="28">
   <si>
     <t>LSP0001</t>
   </si>
@@ -108,6 +96,36 @@
   </si>
   <si>
     <t>pass3</t>
+  </si>
+  <si>
+    <t>Id</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>id_cate</t>
+  </si>
+  <si>
+    <t>SP0001</t>
+  </si>
+  <si>
+    <t>SP0002</t>
+  </si>
+  <si>
+    <t>SP0003</t>
+  </si>
+  <si>
+    <t>SP0004</t>
+  </si>
+  <si>
+    <t>SP0005</t>
+  </si>
+  <si>
+    <t>price</t>
   </si>
 </sst>
 </file>
@@ -118,13 +136,13 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="8"/>
-      <name val="Aptos Narrow"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -488,44 +506,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F06D26A0-5F7D-4EBF-91E8-227E0179787A}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B3" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B4" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>21</v>
       </c>
     </row>
   </sheetData>
@@ -538,17 +557,17 @@
   <dimension ref="A1:B1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>
@@ -558,60 +577,96 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BAB2B3-C2D3-4450-BB20-1F6642B07592}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
+      <c r="D3">
+        <v>20000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="D4">
+        <v>25000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D5">
+        <v>30000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>7</v>
-      </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>9</v>
-      </c>
-      <c r="B6" t="s">
-        <v>13</v>
+      <c r="D6">
+        <v>35000</v>
       </c>
     </row>
   </sheetData>
@@ -627,7 +682,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -639,7 +694,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -651,7 +706,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -665,7 +720,7 @@
       <selection activeCell="I30" sqref="I30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Thêm model và sửa form login
</commit_message>
<xml_diff>
--- a/cafe_management/src/data/dataTemplate.xlsx
+++ b/cafe_management/src/data/dataTemplate.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SPKT\HocKy3\Python\Projects\python\cafe_management\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CF27BFE-823E-4FCE-A754-702AB64CBE66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5E6FE7-99AF-44D3-8BCE-9281376F7AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="2" xr2:uid="{CA152D2A-739E-48A0-B88A-38360C316E83}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CA152D2A-739E-48A0-B88A-38360C316E83}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="7" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>maLSP</t>
   </si>
@@ -108,6 +108,18 @@
   </si>
   <si>
     <t>nameProduct</t>
+  </si>
+  <si>
+    <t>u01</t>
+  </si>
+  <si>
+    <t>u02</t>
+  </si>
+  <si>
+    <t>u03</t>
+  </si>
+  <si>
+    <t>Id</t>
   </si>
 </sst>
 </file>
@@ -488,43 +500,55 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F06D26A0-5F7D-4EBF-91E8-227E0179787A}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I13" sqref="I13"/>
+    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" t="s">
         <v>12</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="C4" s="1" t="s">
         <v>19</v>
       </c>
     </row>
@@ -560,7 +584,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51BAB2B3-C2D3-4450-BB20-1F6642B07592}">
   <dimension ref="A1:B6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Thiết kế giao diện màn hình chính và màn hình quản lý sản phẩm
</commit_message>
<xml_diff>
--- a/cafe_management/src/data/dataTemplate.xlsx
+++ b/cafe_management/src/data/dataTemplate.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SPKT\HocKy3\Python\Projects\python\cafe_management\src\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D5E6FE7-99AF-44D3-8BCE-9281376F7AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{388205D2-2982-4EBB-A30A-155B5FBCA52D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CA152D2A-739E-48A0-B88A-38360C316E83}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>maLSP</t>
   </si>
@@ -86,12 +86,6 @@
     <t>Password</t>
   </si>
   <si>
-    <t>user1</t>
-  </si>
-  <si>
-    <t>pass1</t>
-  </si>
-  <si>
     <t>user2</t>
   </si>
   <si>
@@ -120,6 +114,15 @@
   </si>
   <si>
     <t>Id</t>
+  </si>
+  <si>
+    <t>u1</t>
+  </si>
+  <si>
+    <t>p1</t>
+  </si>
+  <si>
+    <t>u04</t>
   </si>
 </sst>
 </file>
@@ -500,17 +503,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F06D26A0-5F7D-4EBF-91E8-227E0179787A}">
-  <dimension ref="A1:C4"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B1" t="s">
         <v>12</v>
@@ -521,35 +524,46 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>15</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" s="1">
+        <v>1</v>
+      </c>
+      <c r="C5" s="1">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -595,10 +609,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>